<commit_message>
misc download bug fixed
</commit_message>
<xml_diff>
--- a/pub.xlsx
+++ b/pub.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Author nm</t>
   </si>
   <si>
-    <t xml:space="preserve">S R MANI SEKHAR</t>
+    <t xml:space="preserve">Stefan hawking</t>
   </si>
 </sst>
 </file>
@@ -111,11 +111,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -131,15 +131,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
venue and pubshiler now visible
</commit_message>
<xml_diff>
--- a/pub.xlsx
+++ b/pub.xlsx
@@ -20,12 +20,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Author nm</t>
   </si>
   <si>
-    <t xml:space="preserve">Stefan hawking</t>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citation Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cited By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stephan hawking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Journal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security and Privacy Issues in IoT: A Platform for Fog Computing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://scholar.google.co.in/citations?view_op=view_citation&amp;hl=en&amp;user=xew0uSEAAAAJ&amp;citation_for_view=xew0uSEAAAAJ:2osOgNQ5qMEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Journal of Korean Institute of Communications and Information Sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
   </si>
 </sst>
 </file>
@@ -242,10 +278,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -254,10 +290,52 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>